<commit_message>
Har tilføjet %Diff til alle resultater
</commit_message>
<xml_diff>
--- a/Fase3_ValueBettingAnalysis/KNNOutliers/PercentagePointDifference/40pointDifferenceOutliers.xlsx
+++ b/Fase3_ValueBettingAnalysis/KNNOutliers/PercentagePointDifference/40pointDifferenceOutliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE150"/>
+  <dimension ref="A1:AH150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,21 @@
           <t>DiffA</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>%DiffH</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>%DiffD</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>%DiffA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -692,6 +707,15 @@
       <c r="AE2" t="n">
         <v>-0.1392387200440515</v>
       </c>
+      <c r="AF2" t="n">
+        <v>261.8808734230747</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-90.36177304850587</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>-34.98396227006598</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -795,6 +819,15 @@
       <c r="AE3" t="n">
         <v>-0.2194912927044036</v>
       </c>
+      <c r="AF3" t="n">
+        <v>193.5067766979248</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>-91.39852989904119</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>-84.34066324358596</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -898,6 +931,15 @@
       <c r="AE4" t="n">
         <v>-0.1533414718457052</v>
       </c>
+      <c r="AF4" t="n">
+        <v>101.4054559244354</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>-85.6937353705982</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-48.33018138343076</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1001,6 +1043,15 @@
       <c r="AE5" t="n">
         <v>-0.1550886003995883</v>
       </c>
+      <c r="AF5" t="n">
+        <v>189.9623789697343</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>-93.2017343919541</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>-53.8182239374033</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1104,6 +1155,15 @@
       <c r="AE6" t="n">
         <v>-0.1265437007223514</v>
       </c>
+      <c r="AF6" t="n">
+        <v>303.6082434518876</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>-94.6735504029828</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>-26.81258075401753</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1207,6 +1267,15 @@
       <c r="AE7" t="n">
         <v>-0.4334349742683697</v>
       </c>
+      <c r="AF7" t="n">
+        <v>376.146181719355</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-89.64708157335758</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>-73.16398145128964</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1310,6 +1379,15 @@
       <c r="AE8" t="n">
         <v>-0.14666209718085</v>
       </c>
+      <c r="AF8" t="n">
+        <v>103.1627008064253</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>-94.80691900431808</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>-46.96968107711751</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1413,6 +1491,15 @@
       <c r="AE9" t="n">
         <v>-0.2173900289732295</v>
       </c>
+      <c r="AF9" t="n">
+        <v>199.2320175751284</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>-88.32753755093583</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>-77.14487091161547</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1516,6 +1603,15 @@
       <c r="AE10" t="n">
         <v>-0.1762133946199751</v>
       </c>
+      <c r="AF10" t="n">
+        <v>256.8211614598018</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>-86.36668697492451</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>-53.78481682464699</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1619,6 +1715,15 @@
       <c r="AE11" t="n">
         <v>-0.2004266148702343</v>
       </c>
+      <c r="AF11" t="n">
+        <v>108.3181004388837</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>-91.98529662482133</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>-71.72906476736948</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1722,6 +1827,15 @@
       <c r="AE12" t="n">
         <v>-0.1618363980092728</v>
       </c>
+      <c r="AF12" t="n">
+        <v>110.8888087165331</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>-98.38463290501272</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>-51.17477105957412</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1825,6 +1939,15 @@
       <c r="AE13" t="n">
         <v>-0.1662140612409734</v>
       </c>
+      <c r="AF13" t="n">
+        <v>92.49740299373066</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>-91.37493627542835</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>-58.87041874387092</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1928,6 +2051,15 @@
       <c r="AE14" t="n">
         <v>-0.151148106882117</v>
       </c>
+      <c r="AF14" t="n">
+        <v>139.152630813806</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>-94.6689887391053</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>-38.3733707005436</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2031,6 +2163,15 @@
       <c r="AE15" t="n">
         <v>-0.1658122235427448</v>
       </c>
+      <c r="AF15" t="n">
+        <v>123.6387035631475</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>-97.91913004884337</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>-47.91471453135422</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2134,6 +2275,15 @@
       <c r="AE16" t="n">
         <v>-0.09189804905694404</v>
       </c>
+      <c r="AF16" t="n">
+        <v>274.5243826307918</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>-91.68078707415326</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>-21.4634043562029</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2237,6 +2387,15 @@
       <c r="AE17" t="n">
         <v>-0.2050321663382946</v>
       </c>
+      <c r="AF17" t="n">
+        <v>228.3609094170749</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>-92.88601650191526</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>-74.07905406016856</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2340,6 +2499,15 @@
       <c r="AE18" t="n">
         <v>-0.09652251002912515</v>
       </c>
+      <c r="AF18" t="n">
+        <v>255.9834659309093</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>-94.93305538559898</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>-21.70280521691772</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2443,6 +2611,15 @@
       <c r="AE19" t="n">
         <v>-0.1440100194084645</v>
       </c>
+      <c r="AF19" t="n">
+        <v>86.79350076675681</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>-96.67553261142655</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>-58.70799349091939</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2546,6 +2723,15 @@
       <c r="AE20" t="n">
         <v>-0.08438028209636089</v>
       </c>
+      <c r="AF20" t="n">
+        <v>96.86491721866827</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>-94.2895442611528</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>-48.97514475151443</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2649,6 +2835,15 @@
       <c r="AE21" t="n">
         <v>-0.221462641859359</v>
       </c>
+      <c r="AF21" t="n">
+        <v>211.6354706897885</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>-89.74475817717705</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>-74.72340595787426</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2752,6 +2947,15 @@
       <c r="AE22" t="n">
         <v>-0.09765197243551949</v>
       </c>
+      <c r="AF22" t="n">
+        <v>311.0750032889292</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>-92.91572329468202</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>-23.97348879716037</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2855,6 +3059,15 @@
       <c r="AE23" t="n">
         <v>-0.2142835946419435</v>
       </c>
+      <c r="AF23" t="n">
+        <v>339.0720019100143</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>-90.9752779679102</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>-51.71372408027244</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2958,6 +3171,15 @@
       <c r="AE24" t="n">
         <v>-0.1827015067651039</v>
       </c>
+      <c r="AF24" t="n">
+        <v>106.3007012255042</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>-90.376684950814</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>-59.7439648112155</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3061,6 +3283,15 @@
       <c r="AE25" t="n">
         <v>-0.1550717012360302</v>
       </c>
+      <c r="AF25" t="n">
+        <v>175.404566297995</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>-92.09089416560316</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>-31.42844767956922</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3164,6 +3395,15 @@
       <c r="AE26" t="n">
         <v>-0.2532190739151223</v>
       </c>
+      <c r="AF26" t="n">
+        <v>224.1499581170722</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>-99.43319744862757</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>-51.68859345704882</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3267,6 +3507,15 @@
       <c r="AE27" t="n">
         <v>-0.2290582438026678</v>
       </c>
+      <c r="AF27" t="n">
+        <v>146.8560936843534</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>-83.4834793009811</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>-62.76586249903674</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3370,6 +3619,15 @@
       <c r="AE28" t="n">
         <v>-0.2108019145061518</v>
       </c>
+      <c r="AF28" t="n">
+        <v>311.705692251894</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>-93.83987232157619</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>-52.30796975045925</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3473,6 +3731,15 @@
       <c r="AE29" t="n">
         <v>-0.1412232760645049</v>
       </c>
+      <c r="AF29" t="n">
+        <v>247.6322541522165</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>-87.52478194904182</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>-35.71238655306598</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3576,6 +3843,15 @@
       <c r="AE30" t="n">
         <v>-0.1646703546418156</v>
       </c>
+      <c r="AF30" t="n">
+        <v>133.8558711203991</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>-92.55234427560812</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>-42.64471865512417</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3679,6 +3955,15 @@
       <c r="AE31" t="n">
         <v>-0.162990210070887</v>
       </c>
+      <c r="AF31" t="n">
+        <v>277.0747178228872</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>-94.62539114824929</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>-46.4697082287166</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3782,6 +4067,15 @@
       <c r="AE32" t="n">
         <v>-0.137302284242757</v>
       </c>
+      <c r="AF32" t="n">
+        <v>234.0213713020274</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>-88.75726544523889</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>-44.08643482539233</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3885,6 +4179,15 @@
       <c r="AE33" t="n">
         <v>-0.1184105784417144</v>
       </c>
+      <c r="AF33" t="n">
+        <v>163.2624415476318</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>-88.08447624601233</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>-44.33402382712467</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3988,6 +4291,15 @@
       <c r="AE34" t="n">
         <v>-0.1580713930361082</v>
       </c>
+      <c r="AF34" t="n">
+        <v>159.2089727729637</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>-92.73091776065067</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>-32.65512300283104</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4091,6 +4403,15 @@
       <c r="AE35" t="n">
         <v>-0.2098710886663927</v>
       </c>
+      <c r="AF35" t="n">
+        <v>290.727837225237</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>-87.77403788631516</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>-51.08344690446457</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4194,6 +4515,15 @@
       <c r="AE36" t="n">
         <v>-0.1341209189039383</v>
       </c>
+      <c r="AF36" t="n">
+        <v>109.3192422665816</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>-96.91795672864029</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>-39.99754772820999</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4297,6 +4627,15 @@
       <c r="AE37" t="n">
         <v>-0.1695737677872289</v>
       </c>
+      <c r="AF37" t="n">
+        <v>140.7658089786594</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>-97.99500293330161</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>-42.53454219205121</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4400,6 +4739,15 @@
       <c r="AE38" t="n">
         <v>-0.1407271084764372</v>
       </c>
+      <c r="AF38" t="n">
+        <v>112.1949817399139</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>-90.42541213742122</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>-40.08028922603191</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4503,6 +4851,15 @@
       <c r="AE39" t="n">
         <v>-0.1661729808760785</v>
       </c>
+      <c r="AF39" t="n">
+        <v>141.4697974157854</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>-88.99658004949558</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>-40.55753222461302</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4606,6 +4963,15 @@
       <c r="AE40" t="n">
         <v>-0.1750817070190314</v>
       </c>
+      <c r="AF40" t="n">
+        <v>118.6990330542279</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>-86.40228072263268</v>
+      </c>
+      <c r="AH40" t="n">
+        <v>-48.4027973458189</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4709,6 +5075,15 @@
       <c r="AE41" t="n">
         <v>-0.1157332362000568</v>
       </c>
+      <c r="AF41" t="n">
+        <v>252.7145230494907</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>-93.06265820652769</v>
+      </c>
+      <c r="AH41" t="n">
+        <v>-29.78788541938439</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4812,6 +5187,15 @@
       <c r="AE42" t="n">
         <v>-0.1588060272747067</v>
       </c>
+      <c r="AF42" t="n">
+        <v>271.9673863253042</v>
+      </c>
+      <c r="AG42" t="n">
+        <v>-90.51522160416096</v>
+      </c>
+      <c r="AH42" t="n">
+        <v>-43.93490094448102</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4915,6 +5299,15 @@
       <c r="AE43" t="n">
         <v>-0.04930448868456999</v>
       </c>
+      <c r="AF43" t="n">
+        <v>250.1482056805627</v>
+      </c>
+      <c r="AG43" t="n">
+        <v>-94.54037780146311</v>
+      </c>
+      <c r="AH43" t="n">
+        <v>-11.85057155385687</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5018,6 +5411,15 @@
       <c r="AE44" t="n">
         <v>-0.2326434661586784</v>
       </c>
+      <c r="AF44" t="n">
+        <v>131.5324407218797</v>
+      </c>
+      <c r="AG44" t="n">
+        <v>-96.83681357671506</v>
+      </c>
+      <c r="AH44" t="n">
+        <v>-71.12339073805352</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5121,6 +5523,15 @@
       <c r="AE45" t="n">
         <v>-0.06185713252128491</v>
       </c>
+      <c r="AF45" t="n">
+        <v>116.1189804356534</v>
+      </c>
+      <c r="AG45" t="n">
+        <v>-93.30304619320947</v>
+      </c>
+      <c r="AH45" t="n">
+        <v>-32.76728251339141</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5224,6 +5635,15 @@
       <c r="AE46" t="n">
         <v>-0.1287491209707274</v>
       </c>
+      <c r="AF46" t="n">
+        <v>106.2852972854325</v>
+      </c>
+      <c r="AG46" t="n">
+        <v>-95.90062630954152</v>
+      </c>
+      <c r="AH46" t="n">
+        <v>-38.44131822302318</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5327,6 +5747,15 @@
       <c r="AE47" t="n">
         <v>-0.1244387154976426</v>
       </c>
+      <c r="AF47" t="n">
+        <v>123.6947772573902</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>-97.72729321126056</v>
+      </c>
+      <c r="AH47" t="n">
+        <v>-36.31840726490762</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5430,6 +5859,15 @@
       <c r="AE48" t="n">
         <v>-0.1053086881080424</v>
       </c>
+      <c r="AF48" t="n">
+        <v>276.2007406211466</v>
+      </c>
+      <c r="AG48" t="n">
+        <v>-91.71859035245284</v>
+      </c>
+      <c r="AH48" t="n">
+        <v>-27.78480940497407</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5533,6 +5971,15 @@
       <c r="AE49" t="n">
         <v>-0.1111435695913098</v>
       </c>
+      <c r="AF49" t="n">
+        <v>180.9978571261249</v>
+      </c>
+      <c r="AG49" t="n">
+        <v>-95.27854842299925</v>
+      </c>
+      <c r="AH49" t="n">
+        <v>-39.31099669572695</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5636,6 +6083,15 @@
       <c r="AE50" t="n">
         <v>-0.1645289454148611</v>
       </c>
+      <c r="AF50" t="n">
+        <v>116.0186250194259</v>
+      </c>
+      <c r="AG50" t="n">
+        <v>-92.79850258536642</v>
+      </c>
+      <c r="AH50" t="n">
+        <v>-52.63939127418816</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5739,6 +6195,15 @@
       <c r="AE51" t="n">
         <v>-0.1441389611609286</v>
       </c>
+      <c r="AF51" t="n">
+        <v>133.0301377639213</v>
+      </c>
+      <c r="AG51" t="n">
+        <v>-85.39851468071204</v>
+      </c>
+      <c r="AH51" t="n">
+        <v>-38.09583961585684</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5842,6 +6307,15 @@
       <c r="AE52" t="n">
         <v>-0.2381382595605188</v>
       </c>
+      <c r="AF52" t="n">
+        <v>133.2381206411856</v>
+      </c>
+      <c r="AG52" t="n">
+        <v>-87.53103451181403</v>
+      </c>
+      <c r="AH52" t="n">
+        <v>-67.37614733035856</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5945,6 +6419,15 @@
       <c r="AE53" t="n">
         <v>-0.1618419310138713</v>
       </c>
+      <c r="AF53" t="n">
+        <v>108.4893823717891</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>-95.11625109965867</v>
+      </c>
+      <c r="AH53" t="n">
+        <v>-51.29112773272114</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6048,6 +6531,15 @@
       <c r="AE54" t="n">
         <v>-0.1566245847988131</v>
       </c>
+      <c r="AF54" t="n">
+        <v>92.30964539074624</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>-97.73917803105276</v>
+      </c>
+      <c r="AH54" t="n">
+        <v>-60.4479169564568</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6151,6 +6643,15 @@
       <c r="AE55" t="n">
         <v>-0.1235520375938892</v>
       </c>
+      <c r="AF55" t="n">
+        <v>120.1239959171884</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>-96.69462753998341</v>
+      </c>
+      <c r="AH55" t="n">
+        <v>-32.87934945999971</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6254,6 +6755,15 @@
       <c r="AE56" t="n">
         <v>-0.1560767354175827</v>
       </c>
+      <c r="AF56" t="n">
+        <v>118.7755809668114</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>-93.02277951895465</v>
+      </c>
+      <c r="AH56" t="n">
+        <v>-42.65606378833467</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6357,6 +6867,15 @@
       <c r="AE57" t="n">
         <v>-0.1683616619325881</v>
       </c>
+      <c r="AF57" t="n">
+        <v>106.6256167928453</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>-95.90764522258046</v>
+      </c>
+      <c r="AH57" t="n">
+        <v>-58.25454075722284</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6460,6 +6979,15 @@
       <c r="AE58" t="n">
         <v>-0.2456388070673214</v>
       </c>
+      <c r="AF58" t="n">
+        <v>261.8897941494533</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>-82.6634022810177</v>
+      </c>
+      <c r="AH58" t="n">
+        <v>-68.35626731399722</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6563,6 +7091,15 @@
       <c r="AE59" t="n">
         <v>-0.1786291457506457</v>
       </c>
+      <c r="AF59" t="n">
+        <v>118.0637465408066</v>
+      </c>
+      <c r="AG59" t="n">
+        <v>-87.7456247360371</v>
+      </c>
+      <c r="AH59" t="n">
+        <v>-51.0663386213775</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6666,6 +7203,15 @@
       <c r="AE60" t="n">
         <v>-0.1748846393841797</v>
       </c>
+      <c r="AF60" t="n">
+        <v>147.7343581663232</v>
+      </c>
+      <c r="AG60" t="n">
+        <v>-98.44078306450254</v>
+      </c>
+      <c r="AH60" t="n">
+        <v>-42.57074111576777</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6769,6 +7315,15 @@
       <c r="AE61" t="n">
         <v>-0.2036162516759085</v>
       </c>
+      <c r="AF61" t="n">
+        <v>123.2891292494501</v>
+      </c>
+      <c r="AG61" t="n">
+        <v>-90.73255759389586</v>
+      </c>
+      <c r="AH61" t="n">
+        <v>-65.54976599044333</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6872,6 +7427,15 @@
       <c r="AE62" t="n">
         <v>-0.1442084739457307</v>
       </c>
+      <c r="AF62" t="n">
+        <v>214.182104475733</v>
+      </c>
+      <c r="AG62" t="n">
+        <v>-90.3794195006073</v>
+      </c>
+      <c r="AH62" t="n">
+        <v>-46.50870250355023</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6975,6 +7539,15 @@
       <c r="AE63" t="n">
         <v>-0.1949391230037612</v>
       </c>
+      <c r="AF63" t="n">
+        <v>176.5982549368377</v>
+      </c>
+      <c r="AG63" t="n">
+        <v>-90.84717698752023</v>
+      </c>
+      <c r="AH63" t="n">
+        <v>-76.26268766776583</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -7078,6 +7651,15 @@
       <c r="AE64" t="n">
         <v>-0.1672878027175711</v>
       </c>
+      <c r="AF64" t="n">
+        <v>108.5514197420066</v>
+      </c>
+      <c r="AG64" t="n">
+        <v>-98.33369606870653</v>
+      </c>
+      <c r="AH64" t="n">
+        <v>-55.93657074111083</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7181,6 +7763,15 @@
       <c r="AE65" t="n">
         <v>-0.07301311694132423</v>
       </c>
+      <c r="AF65" t="n">
+        <v>186.3469281406134</v>
+      </c>
+      <c r="AG65" t="n">
+        <v>-88.57286528407037</v>
+      </c>
+      <c r="AH65" t="n">
+        <v>-28.11829214961889</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7284,6 +7875,15 @@
       <c r="AE66" t="n">
         <v>-0.1920151140143813</v>
       </c>
+      <c r="AF66" t="n">
+        <v>242.2426143009748</v>
+      </c>
+      <c r="AG66" t="n">
+        <v>-88.44235674390052</v>
+      </c>
+      <c r="AH66" t="n">
+        <v>-55.91543904870636</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7387,6 +7987,15 @@
       <c r="AE67" t="n">
         <v>-0.1873477652308767</v>
       </c>
+      <c r="AF67" t="n">
+        <v>126.1128025100214</v>
+      </c>
+      <c r="AG67" t="n">
+        <v>-97.78877607287605</v>
+      </c>
+      <c r="AH67" t="n">
+        <v>-52.03383693182491</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7490,6 +8099,15 @@
       <c r="AE68" t="n">
         <v>-0.1501046815555685</v>
       </c>
+      <c r="AF68" t="n">
+        <v>87.96166894418455</v>
+      </c>
+      <c r="AG68" t="n">
+        <v>-91.60200119734738</v>
+      </c>
+      <c r="AH68" t="n">
+        <v>-58.24110179500938</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7593,6 +8211,15 @@
       <c r="AE69" t="n">
         <v>-0.1817639295289987</v>
       </c>
+      <c r="AF69" t="n">
+        <v>117.2608520168391</v>
+      </c>
+      <c r="AG69" t="n">
+        <v>-90.6212994859938</v>
+      </c>
+      <c r="AH69" t="n">
+        <v>-52.4740151330488</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7696,6 +8323,15 @@
       <c r="AE70" t="n">
         <v>-0.115622719570749</v>
       </c>
+      <c r="AF70" t="n">
+        <v>141.236184116541</v>
+      </c>
+      <c r="AG70" t="n">
+        <v>-92.42999412255605</v>
+      </c>
+      <c r="AH70" t="n">
+        <v>-50.98258809044356</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7799,6 +8435,15 @@
       <c r="AE71" t="n">
         <v>-0.1111177938152717</v>
       </c>
+      <c r="AF71" t="n">
+        <v>183.5197405539994</v>
+      </c>
+      <c r="AG71" t="n">
+        <v>-86.64656057187854</v>
+      </c>
+      <c r="AH71" t="n">
+        <v>-39.84804649568701</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7902,6 +8547,15 @@
       <c r="AE72" t="n">
         <v>-0.1270019742368936</v>
       </c>
+      <c r="AF72" t="n">
+        <v>275.8830799435723</v>
+      </c>
+      <c r="AG72" t="n">
+        <v>-91.61673194677059</v>
+      </c>
+      <c r="AH72" t="n">
+        <v>-34.90382788273812</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -8005,6 +8659,15 @@
       <c r="AE73" t="n">
         <v>-0.1412087549670051</v>
       </c>
+      <c r="AF73" t="n">
+        <v>107.9354456938421</v>
+      </c>
+      <c r="AG73" t="n">
+        <v>-96.36570955506058</v>
+      </c>
+      <c r="AH73" t="n">
+        <v>-42.37820460997641</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -8108,6 +8771,15 @@
       <c r="AE74" t="n">
         <v>-0.111060479777515</v>
       </c>
+      <c r="AF74" t="n">
+        <v>269.8411176605303</v>
+      </c>
+      <c r="AG74" t="n">
+        <v>-88.41776628974617</v>
+      </c>
+      <c r="AH74" t="n">
+        <v>-25.12235332353819</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -8211,6 +8883,15 @@
       <c r="AE75" t="n">
         <v>-0.02383113957748179</v>
       </c>
+      <c r="AF75" t="n">
+        <v>241.9241654386376</v>
+      </c>
+      <c r="AG75" t="n">
+        <v>-96.2652010400453</v>
+      </c>
+      <c r="AH75" t="n">
+        <v>-5.388485016416694</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -8314,6 +8995,15 @@
       <c r="AE76" t="n">
         <v>-0.164766560308391</v>
       </c>
+      <c r="AF76" t="n">
+        <v>88.69472715537587</v>
+      </c>
+      <c r="AG76" t="n">
+        <v>-97.21133973459089</v>
+      </c>
+      <c r="AH76" t="n">
+        <v>-70.56919390525645</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -8417,6 +9107,15 @@
       <c r="AE77" t="n">
         <v>-0.1371606438352105</v>
       </c>
+      <c r="AF77" t="n">
+        <v>311.6990454217843</v>
+      </c>
+      <c r="AG77" t="n">
+        <v>-94.40067112611048</v>
+      </c>
+      <c r="AH77" t="n">
+        <v>-27.42991422025145</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8520,6 +9219,15 @@
       <c r="AE78" t="n">
         <v>-0.05417633434400992</v>
       </c>
+      <c r="AF78" t="n">
+        <v>254.6656562310012</v>
+      </c>
+      <c r="AG78" t="n">
+        <v>-93.45977029006683</v>
+      </c>
+      <c r="AH78" t="n">
+        <v>-11.97322763703102</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8623,6 +9331,15 @@
       <c r="AE79" t="n">
         <v>-0.1991016603996554</v>
       </c>
+      <c r="AF79" t="n">
+        <v>119.7182376514147</v>
+      </c>
+      <c r="AG79" t="n">
+        <v>-98.33231290875852</v>
+      </c>
+      <c r="AH79" t="n">
+        <v>-64.51925353325076</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8726,6 +9443,15 @@
       <c r="AE80" t="n">
         <v>-0.04968117774156328</v>
       </c>
+      <c r="AF80" t="n">
+        <v>243.84313139149</v>
+      </c>
+      <c r="AG80" t="n">
+        <v>-94.38185076746915</v>
+      </c>
+      <c r="AH80" t="n">
+        <v>-10.98573419187764</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8829,6 +9555,15 @@
       <c r="AE81" t="n">
         <v>-0.1260855030508602</v>
       </c>
+      <c r="AF81" t="n">
+        <v>102.1619771809367</v>
+      </c>
+      <c r="AG81" t="n">
+        <v>-94.71299967761408</v>
+      </c>
+      <c r="AH81" t="n">
+        <v>-39.88738804306182</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -8932,6 +9667,15 @@
       <c r="AE82" t="n">
         <v>-0.2344811894294823</v>
       </c>
+      <c r="AF82" t="n">
+        <v>367.4019808929128</v>
+      </c>
+      <c r="AG82" t="n">
+        <v>-89.24634136561629</v>
+      </c>
+      <c r="AH82" t="n">
+        <v>-59.31013790089549</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -9035,6 +9779,15 @@
       <c r="AE83" t="n">
         <v>-0.0920059604113527</v>
       </c>
+      <c r="AF83" t="n">
+        <v>210.8182737937491</v>
+      </c>
+      <c r="AG83" t="n">
+        <v>-89.24213406471141</v>
+      </c>
+      <c r="AH83" t="n">
+        <v>-31.23297279904978</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -9138,6 +9891,15 @@
       <c r="AE84" t="n">
         <v>-0.1359950118690802</v>
       </c>
+      <c r="AF84" t="n">
+        <v>242.6350160246483</v>
+      </c>
+      <c r="AG84" t="n">
+        <v>-89.41497700893134</v>
+      </c>
+      <c r="AH84" t="n">
+        <v>-41.96668509543751</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -9241,6 +10003,15 @@
       <c r="AE85" t="n">
         <v>-0.1812402079678075</v>
       </c>
+      <c r="AF85" t="n">
+        <v>322.1288059541886</v>
+      </c>
+      <c r="AG85" t="n">
+        <v>-87.57071627901814</v>
+      </c>
+      <c r="AH85" t="n">
+        <v>-44.7545117511434</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -9344,6 +10115,15 @@
       <c r="AE86" t="n">
         <v>-0.1712775061101476</v>
       </c>
+      <c r="AF86" t="n">
+        <v>329.1155769941539</v>
+      </c>
+      <c r="AG86" t="n">
+        <v>-85.92549778231641</v>
+      </c>
+      <c r="AH86" t="n">
+        <v>-43.97530844484993</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -9447,6 +10227,15 @@
       <c r="AE87" t="n">
         <v>-0.151377646613079</v>
       </c>
+      <c r="AF87" t="n">
+        <v>113.7172543303104</v>
+      </c>
+      <c r="AG87" t="n">
+        <v>-91.50128602500496</v>
+      </c>
+      <c r="AH87" t="n">
+        <v>-41.62238368839958</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -9550,6 +10339,15 @@
       <c r="AE88" t="n">
         <v>-0.1450274784866966</v>
       </c>
+      <c r="AF88" t="n">
+        <v>325.716222046749</v>
+      </c>
+      <c r="AG88" t="n">
+        <v>-96.01599930909272</v>
+      </c>
+      <c r="AH88" t="n">
+        <v>-26.41716384521266</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -9653,6 +10451,15 @@
       <c r="AE89" t="n">
         <v>-0.1189160742106422</v>
       </c>
+      <c r="AF89" t="n">
+        <v>194.5052874776479</v>
+      </c>
+      <c r="AG89" t="n">
+        <v>-95.29776635192152</v>
+      </c>
+      <c r="AH89" t="n">
+        <v>-39.06261590513967</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -9756,6 +10563,15 @@
       <c r="AE90" t="n">
         <v>-0.1075115143147909</v>
       </c>
+      <c r="AF90" t="n">
+        <v>196.8572419465419</v>
+      </c>
+      <c r="AG90" t="n">
+        <v>-88.25182925843784</v>
+      </c>
+      <c r="AH90" t="n">
+        <v>-39.81373284404977</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -9859,6 +10675,15 @@
       <c r="AE91" t="n">
         <v>-0.1340494903276389</v>
       </c>
+      <c r="AF91" t="n">
+        <v>106.9819904506899</v>
+      </c>
+      <c r="AG91" t="n">
+        <v>-98.49042678801091</v>
+      </c>
+      <c r="AH91" t="n">
+        <v>-42.2965091917217</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -9962,6 +10787,15 @@
       <c r="AE92" t="n">
         <v>-0.1445627028114518</v>
       </c>
+      <c r="AF92" t="n">
+        <v>112.4618686405876</v>
+      </c>
+      <c r="AG92" t="n">
+        <v>-87.8128769472942</v>
+      </c>
+      <c r="AH92" t="n">
+        <v>-41.28191261610978</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -10065,6 +10899,15 @@
       <c r="AE93" t="n">
         <v>-0.2150567370076746</v>
       </c>
+      <c r="AF93" t="n">
+        <v>137.2129067073658</v>
+      </c>
+      <c r="AG93" t="n">
+        <v>-82.38868201009112</v>
+      </c>
+      <c r="AH93" t="n">
+        <v>-49.23203754701916</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -10168,6 +11011,15 @@
       <c r="AE94" t="n">
         <v>-0.1554579164038642</v>
       </c>
+      <c r="AF94" t="n">
+        <v>86.29944570801324</v>
+      </c>
+      <c r="AG94" t="n">
+        <v>-95.71601820481034</v>
+      </c>
+      <c r="AH94" t="n">
+        <v>-68.36429098355376</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -10271,6 +11123,15 @@
       <c r="AE95" t="n">
         <v>-0.1431194013341655</v>
       </c>
+      <c r="AF95" t="n">
+        <v>92.05027625288736</v>
+      </c>
+      <c r="AG95" t="n">
+        <v>-96.88567695487124</v>
+      </c>
+      <c r="AH95" t="n">
+        <v>-56.20627095577445</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -10374,6 +11235,15 @@
       <c r="AE96" t="n">
         <v>-0.1818632369869854</v>
       </c>
+      <c r="AF96" t="n">
+        <v>237.2841103314693</v>
+      </c>
+      <c r="AG96" t="n">
+        <v>-87.39030151799602</v>
+      </c>
+      <c r="AH96" t="n">
+        <v>-45.79190208237866</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -10477,6 +11347,15 @@
       <c r="AE97" t="n">
         <v>-0.09753651097814214</v>
       </c>
+      <c r="AF97" t="n">
+        <v>290.1014565453257</v>
+      </c>
+      <c r="AG97" t="n">
+        <v>-92.57293455922066</v>
+      </c>
+      <c r="AH97" t="n">
+        <v>-21.28483963558341</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -10580,6 +11459,15 @@
       <c r="AE98" t="n">
         <v>-0.1193054560189128</v>
       </c>
+      <c r="AF98" t="n">
+        <v>155.6996652736771</v>
+      </c>
+      <c r="AG98" t="n">
+        <v>-94.89031083160977</v>
+      </c>
+      <c r="AH98" t="n">
+        <v>-27.92118167934366</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -10683,6 +11571,15 @@
       <c r="AE99" t="n">
         <v>-0.1319175477201974</v>
       </c>
+      <c r="AF99" t="n">
+        <v>102.7047190533468</v>
+      </c>
+      <c r="AG99" t="n">
+        <v>-93.11317561199407</v>
+      </c>
+      <c r="AH99" t="n">
+        <v>-41.29270513039526</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -10786,6 +11683,15 @@
       <c r="AE100" t="n">
         <v>-0.1445910746024546</v>
       </c>
+      <c r="AF100" t="n">
+        <v>104.0784920952523</v>
+      </c>
+      <c r="AG100" t="n">
+        <v>-91.10688344384526</v>
+      </c>
+      <c r="AH100" t="n">
+        <v>-44.47634424712893</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -10889,6 +11795,15 @@
       <c r="AE101" t="n">
         <v>-0.1659496789403619</v>
       </c>
+      <c r="AF101" t="n">
+        <v>101.6636884695343</v>
+      </c>
+      <c r="AG101" t="n">
+        <v>-95.72253140128079</v>
+      </c>
+      <c r="AH101" t="n">
+        <v>-58.7511461338435</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -10992,6 +11907,15 @@
       <c r="AE102" t="n">
         <v>-0.1371256610990849</v>
       </c>
+      <c r="AF102" t="n">
+        <v>100.758620907181</v>
+      </c>
+      <c r="AG102" t="n">
+        <v>-93.04334683697138</v>
+      </c>
+      <c r="AH102" t="n">
+        <v>-43.99072762239808</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -11095,6 +12019,15 @@
       <c r="AE103" t="n">
         <v>-0.2420425486389554</v>
       </c>
+      <c r="AF103" t="n">
+        <v>263.8510634991391</v>
+      </c>
+      <c r="AG103" t="n">
+        <v>-97.22809558604033</v>
+      </c>
+      <c r="AH103" t="n">
+        <v>-43.52834949028629</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -11198,6 +12131,15 @@
       <c r="AE104" t="n">
         <v>-0.177548064073078</v>
       </c>
+      <c r="AF104" t="n">
+        <v>111.4071146577759</v>
+      </c>
+      <c r="AG104" t="n">
+        <v>-95.86045534892833</v>
+      </c>
+      <c r="AH104" t="n">
+        <v>-57.30314118052532</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -11301,6 +12243,15 @@
       <c r="AE105" t="n">
         <v>-0.1467688754512692</v>
       </c>
+      <c r="AF105" t="n">
+        <v>90.68211264547907</v>
+      </c>
+      <c r="AG105" t="n">
+        <v>-93.51888580555242</v>
+      </c>
+      <c r="AH105" t="n">
+        <v>-53.76061565587409</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -11404,6 +12355,15 @@
       <c r="AE106" t="n">
         <v>-0.1739157258655598</v>
       </c>
+      <c r="AF106" t="n">
+        <v>138.7212513060598</v>
+      </c>
+      <c r="AG106" t="n">
+        <v>-86.25739678093531</v>
+      </c>
+      <c r="AH106" t="n">
+        <v>-72.22711403888286</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -11507,6 +12467,15 @@
       <c r="AE107" t="n">
         <v>-0.09008889785258357</v>
       </c>
+      <c r="AF107" t="n">
+        <v>104.8922174637029</v>
+      </c>
+      <c r="AG107" t="n">
+        <v>-87.36845721647968</v>
+      </c>
+      <c r="AH107" t="n">
+        <v>-51.94866129245334</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -11610,6 +12579,15 @@
       <c r="AE108" t="n">
         <v>-0.1344237327134988</v>
       </c>
+      <c r="AF108" t="n">
+        <v>84.54842778683198</v>
+      </c>
+      <c r="AG108" t="n">
+        <v>-93.91777255143434</v>
+      </c>
+      <c r="AH108" t="n">
+        <v>-56.9202266279024</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -11713,6 +12691,15 @@
       <c r="AE109" t="n">
         <v>-0.1383082647265025</v>
       </c>
+      <c r="AF109" t="n">
+        <v>96.09866130733248</v>
+      </c>
+      <c r="AG109" t="n">
+        <v>-96.76397802875292</v>
+      </c>
+      <c r="AH109" t="n">
+        <v>-49.01818836183903</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -11816,6 +12803,15 @@
       <c r="AE110" t="n">
         <v>-0.1686142863271605</v>
       </c>
+      <c r="AF110" t="n">
+        <v>139.1169254365805</v>
+      </c>
+      <c r="AG110" t="n">
+        <v>-91.98110918677261</v>
+      </c>
+      <c r="AH110" t="n">
+        <v>-45.64833357051351</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -11919,6 +12915,15 @@
       <c r="AE111" t="n">
         <v>-0.1735502701757607</v>
       </c>
+      <c r="AF111" t="n">
+        <v>270.2554003858643</v>
+      </c>
+      <c r="AG111" t="n">
+        <v>-92.06770804293187</v>
+      </c>
+      <c r="AH111" t="n">
+        <v>-39.74470862931712</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -12022,6 +13027,15 @@
       <c r="AE112" t="n">
         <v>-0.2285108615769637</v>
       </c>
+      <c r="AF112" t="n">
+        <v>321.3234363524414</v>
+      </c>
+      <c r="AG112" t="n">
+        <v>-90.30526312158544</v>
+      </c>
+      <c r="AH112" t="n">
+        <v>-57.96141144751466</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -12125,6 +13139,15 @@
       <c r="AE113" t="n">
         <v>-0.1068301360833998</v>
       </c>
+      <c r="AF113" t="n">
+        <v>318.0490209878431</v>
+      </c>
+      <c r="AG113" t="n">
+        <v>-95.4273315565288</v>
+      </c>
+      <c r="AH113" t="n">
+        <v>-20.93479628598546</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -12228,6 +13251,15 @@
       <c r="AE114" t="n">
         <v>-0.006026039482317502</v>
       </c>
+      <c r="AF114" t="n">
+        <v>160.7342209690823</v>
+      </c>
+      <c r="AG114" t="n">
+        <v>-96.08529647664979</v>
+      </c>
+      <c r="AH114" t="n">
+        <v>-1.926950916064191</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -12331,6 +13363,15 @@
       <c r="AE115" t="n">
         <v>-0.1877532692125904</v>
       </c>
+      <c r="AF115" t="n">
+        <v>325.3558152013936</v>
+      </c>
+      <c r="AG115" t="n">
+        <v>-89.86913852753439</v>
+      </c>
+      <c r="AH115" t="n">
+        <v>-41.65664756921407</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -12434,6 +13475,15 @@
       <c r="AE116" t="n">
         <v>-0.1057630619276278</v>
       </c>
+      <c r="AF116" t="n">
+        <v>113.0401222168727</v>
+      </c>
+      <c r="AG116" t="n">
+        <v>-92.81337474079353</v>
+      </c>
+      <c r="AH116" t="n">
+        <v>-55.80267791923468</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -12537,6 +13587,15 @@
       <c r="AE117" t="n">
         <v>-0.1323081164607265</v>
       </c>
+      <c r="AF117" t="n">
+        <v>121.6400353411528</v>
+      </c>
+      <c r="AG117" t="n">
+        <v>-93.24044846334142</v>
+      </c>
+      <c r="AH117" t="n">
+        <v>-35.06803640333298</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -12640,6 +13699,15 @@
       <c r="AE118" t="n">
         <v>-0.1937847306554591</v>
       </c>
+      <c r="AF118" t="n">
+        <v>114.5001968730434</v>
+      </c>
+      <c r="AG118" t="n">
+        <v>-90.50620360133308</v>
+      </c>
+      <c r="AH118" t="n">
+        <v>-58.26780933027577</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -12743,6 +13811,15 @@
       <c r="AE119" t="n">
         <v>-0.2788028231275417</v>
       </c>
+      <c r="AF119" t="n">
+        <v>134.6280730264819</v>
+      </c>
+      <c r="AG119" t="n">
+        <v>-84.00997084487794</v>
+      </c>
+      <c r="AH119" t="n">
+        <v>-67.79269420736149</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -12846,6 +13923,15 @@
       <c r="AE120" t="n">
         <v>-0.1884731914802461</v>
       </c>
+      <c r="AF120" t="n">
+        <v>139.190008650188</v>
+      </c>
+      <c r="AG120" t="n">
+        <v>-91.36340344475512</v>
+      </c>
+      <c r="AH120" t="n">
+        <v>-48.98136962796129</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -12949,6 +14035,15 @@
       <c r="AE121" t="n">
         <v>-0.1811727388809055</v>
       </c>
+      <c r="AF121" t="n">
+        <v>101.183536171429</v>
+      </c>
+      <c r="AG121" t="n">
+        <v>-97.2715391515877</v>
+      </c>
+      <c r="AH121" t="n">
+        <v>-67.75774773276419</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -13052,6 +14147,15 @@
       <c r="AE122" t="n">
         <v>-0.1492410716002069</v>
       </c>
+      <c r="AF122" t="n">
+        <v>96.25471128836017</v>
+      </c>
+      <c r="AG122" t="n">
+        <v>-97.35424923739575</v>
+      </c>
+      <c r="AH122" t="n">
+        <v>-54.43089613437721</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -13155,6 +14259,15 @@
       <c r="AE123" t="n">
         <v>-0.1434498697672295</v>
       </c>
+      <c r="AF123" t="n">
+        <v>97.64731527416885</v>
+      </c>
+      <c r="AG123" t="n">
+        <v>-95.73098997386552</v>
+      </c>
+      <c r="AH123" t="n">
+        <v>-48.9237866801211</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -13258,6 +14371,15 @@
       <c r="AE124" t="n">
         <v>-0.1469651883201769</v>
       </c>
+      <c r="AF124" t="n">
+        <v>294.2499264926757</v>
+      </c>
+      <c r="AG124" t="n">
+        <v>-91.69113388285511</v>
+      </c>
+      <c r="AH124" t="n">
+        <v>-29.5100945412149</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -13361,6 +14483,15 @@
       <c r="AE125" t="n">
         <v>-0.162844641639344</v>
       </c>
+      <c r="AF125" t="n">
+        <v>140.5241239248077</v>
+      </c>
+      <c r="AG125" t="n">
+        <v>-92.70438445015662</v>
+      </c>
+      <c r="AH125" t="n">
+        <v>-38.29252948877208</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -13464,6 +14595,15 @@
       <c r="AE126" t="n">
         <v>-0.2244460084689166</v>
       </c>
+      <c r="AF126" t="n">
+        <v>289.1021330839963</v>
+      </c>
+      <c r="AG126" t="n">
+        <v>-93.63287636416443</v>
+      </c>
+      <c r="AH126" t="n">
+        <v>-35.69061679782873</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -13567,6 +14707,15 @@
       <c r="AE127" t="n">
         <v>-0.1091654443096691</v>
       </c>
+      <c r="AF127" t="n">
+        <v>272.534721322939</v>
+      </c>
+      <c r="AG127" t="n">
+        <v>-94.75176009303716</v>
+      </c>
+      <c r="AH127" t="n">
+        <v>-30.7420311204459</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -13670,6 +14819,15 @@
       <c r="AE128" t="n">
         <v>-0.157905149796894</v>
       </c>
+      <c r="AF128" t="n">
+        <v>116.923727600666</v>
+      </c>
+      <c r="AG128" t="n">
+        <v>-92.29639229715112</v>
+      </c>
+      <c r="AH128" t="n">
+        <v>-45.458999430101</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -13773,6 +14931,15 @@
       <c r="AE129" t="n">
         <v>-0.1674489099473842</v>
       </c>
+      <c r="AF129" t="n">
+        <v>117.053656257576</v>
+      </c>
+      <c r="AG129" t="n">
+        <v>-98.96779921121542</v>
+      </c>
+      <c r="AH129" t="n">
+        <v>-49.89104273791261</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -13876,6 +15043,15 @@
       <c r="AE130" t="n">
         <v>-0.0247224408180913</v>
       </c>
+      <c r="AF130" t="n">
+        <v>103.7214731575149</v>
+      </c>
+      <c r="AG130" t="n">
+        <v>-97.36932601745359</v>
+      </c>
+      <c r="AH130" t="n">
+        <v>-11.60843931842911</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -13979,6 +15155,15 @@
       <c r="AE131" t="n">
         <v>-0.1312040043200091</v>
       </c>
+      <c r="AF131" t="n">
+        <v>113.8699772968819</v>
+      </c>
+      <c r="AG131" t="n">
+        <v>-99.06948607664631</v>
+      </c>
+      <c r="AH131" t="n">
+        <v>-39.20655751372246</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -14082,6 +15267,15 @@
       <c r="AE132" t="n">
         <v>-0.1237807511305277</v>
       </c>
+      <c r="AF132" t="n">
+        <v>107.1538042345775</v>
+      </c>
+      <c r="AG132" t="n">
+        <v>-97.96152382422638</v>
+      </c>
+      <c r="AH132" t="n">
+        <v>-36.55186065804549</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -14185,6 +15379,15 @@
       <c r="AE133" t="n">
         <v>-0.1519570010877229</v>
       </c>
+      <c r="AF133" t="n">
+        <v>143.3092537358864</v>
+      </c>
+      <c r="AG133" t="n">
+        <v>-92.65800820913908</v>
+      </c>
+      <c r="AH133" t="n">
+        <v>-36.25053161736151</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -14288,6 +15491,15 @@
       <c r="AE134" t="n">
         <v>-0.1484543449327288</v>
       </c>
+      <c r="AF134" t="n">
+        <v>250.4258121578041</v>
+      </c>
+      <c r="AG134" t="n">
+        <v>-94.80429110104141</v>
+      </c>
+      <c r="AH134" t="n">
+        <v>-43.97332741069378</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -14391,6 +15603,15 @@
       <c r="AE135" t="n">
         <v>-0.1916344429980365</v>
       </c>
+      <c r="AF135" t="n">
+        <v>112.7932794997558</v>
+      </c>
+      <c r="AG135" t="n">
+        <v>-98.9448816828386</v>
+      </c>
+      <c r="AH135" t="n">
+        <v>-64.88957406588938</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -14494,6 +15715,15 @@
       <c r="AE136" t="n">
         <v>-0.1431319287023629</v>
       </c>
+      <c r="AF136" t="n">
+        <v>154.38825370788</v>
+      </c>
+      <c r="AG136" t="n">
+        <v>-89.25646941425441</v>
+      </c>
+      <c r="AH136" t="n">
+        <v>-64.0757718791136</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -14597,6 +15827,15 @@
       <c r="AE137" t="n">
         <v>-0.1466288468577288</v>
       </c>
+      <c r="AF137" t="n">
+        <v>125.5781043097012</v>
+      </c>
+      <c r="AG137" t="n">
+        <v>-96.23479052490485</v>
+      </c>
+      <c r="AH137" t="n">
+        <v>-45.456680016919</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -14700,6 +15939,15 @@
       <c r="AE138" t="n">
         <v>-0.1293233032684488</v>
       </c>
+      <c r="AF138" t="n">
+        <v>105.6050124698112</v>
+      </c>
+      <c r="AG138" t="n">
+        <v>-98.95336001089061</v>
+      </c>
+      <c r="AH138" t="n">
+        <v>-39.74562580309683</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -14803,6 +16051,15 @@
       <c r="AE139" t="n">
         <v>-0.1191106773175468</v>
       </c>
+      <c r="AF139" t="n">
+        <v>290.0115021202805</v>
+      </c>
+      <c r="AG139" t="n">
+        <v>-95.81353111231955</v>
+      </c>
+      <c r="AH139" t="n">
+        <v>-26.11144369426515</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -14906,6 +16163,15 @@
       <c r="AE140" t="n">
         <v>-0.1921350922662425</v>
       </c>
+      <c r="AF140" t="n">
+        <v>188.6612181665495</v>
+      </c>
+      <c r="AG140" t="n">
+        <v>-97.18008219865327</v>
+      </c>
+      <c r="AH140" t="n">
+        <v>-41.5042106426806</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -15009,6 +16275,15 @@
       <c r="AE141" t="n">
         <v>-0.1628628302202025</v>
       </c>
+      <c r="AF141" t="n">
+        <v>131.5287133669208</v>
+      </c>
+      <c r="AG141" t="n">
+        <v>-90.80858525489398</v>
+      </c>
+      <c r="AH141" t="n">
+        <v>-45.4752027083569</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -15112,6 +16387,15 @@
       <c r="AE142" t="n">
         <v>-0.1399515575383138</v>
       </c>
+      <c r="AF142" t="n">
+        <v>328.8856734831505</v>
+      </c>
+      <c r="AG142" t="n">
+        <v>-95.42011107682474</v>
+      </c>
+      <c r="AH142" t="n">
+        <v>-27.8122409074923</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -15215,6 +16499,15 @@
       <c r="AE143" t="n">
         <v>-0.1427939733805882</v>
       </c>
+      <c r="AF143" t="n">
+        <v>84.27944687412209</v>
+      </c>
+      <c r="AG143" t="n">
+        <v>-92.61948158330038</v>
+      </c>
+      <c r="AH143" t="n">
+        <v>-58.76251298296488</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -15318,6 +16611,15 @@
       <c r="AE144" t="n">
         <v>-0.1648396983570939</v>
       </c>
+      <c r="AF144" t="n">
+        <v>132.3123128041287</v>
+      </c>
+      <c r="AG144" t="n">
+        <v>-86.93828778894165</v>
+      </c>
+      <c r="AH144" t="n">
+        <v>-82.81855035184394</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -15421,6 +16723,15 @@
       <c r="AE145" t="n">
         <v>-0.1303886944337121</v>
       </c>
+      <c r="AF145" t="n">
+        <v>121.8969326344999</v>
+      </c>
+      <c r="AG145" t="n">
+        <v>-97.5602482387866</v>
+      </c>
+      <c r="AH145" t="n">
+        <v>-35.59259945815628</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -15524,6 +16835,15 @@
       <c r="AE146" t="n">
         <v>-0.1689703462316599</v>
       </c>
+      <c r="AF146" t="n">
+        <v>120.2650509819533</v>
+      </c>
+      <c r="AG146" t="n">
+        <v>-98.39733840912005</v>
+      </c>
+      <c r="AH146" t="n">
+        <v>-50.8275325034212</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -15627,6 +16947,15 @@
       <c r="AE147" t="n">
         <v>-0.1462451576450303</v>
       </c>
+      <c r="AF147" t="n">
+        <v>158.6718060195995</v>
+      </c>
+      <c r="AG147" t="n">
+        <v>-93.73366876608624</v>
+      </c>
+      <c r="AH147" t="n">
+        <v>-31.79145996399149</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -15730,6 +17059,15 @@
       <c r="AE148" t="n">
         <v>-0.146150825204133</v>
       </c>
+      <c r="AF148" t="n">
+        <v>102.0778413393567</v>
+      </c>
+      <c r="AG148" t="n">
+        <v>-96.20332649897782</v>
+      </c>
+      <c r="AH148" t="n">
+        <v>-49.81195154792167</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -15833,6 +17171,15 @@
       <c r="AE149" t="n">
         <v>-0.2497316971733656</v>
       </c>
+      <c r="AF149" t="n">
+        <v>201.2840985848103</v>
+      </c>
+      <c r="AG149" t="n">
+        <v>-90.07435133304864</v>
+      </c>
+      <c r="AH149" t="n">
+        <v>-52.16246282722091</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -15935,6 +17282,15 @@
       </c>
       <c r="AE150" t="n">
         <v>-0.172290023786222</v>
+      </c>
+      <c r="AF150" t="n">
+        <v>302.5597652971716</v>
+      </c>
+      <c r="AG150" t="n">
+        <v>-90.31276203718144</v>
+      </c>
+      <c r="AH150" t="n">
+        <v>-40.70025732320579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>